<commit_message>
Adding CarBase class, adding parameterization, getting title of the page
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rimadas/eclipse-workspace/SeleniumDataDrivenFramework/src/test/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rimadas/eclipse-workspace/SeleniumPageObjectModelFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E758EBCB-2BE0-C649-9FD5-0D622B894F4A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B03991-E471-F54F-A3CC-48A0FF32A590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22820" yWindow="1460" windowWidth="12620" windowHeight="10360" activeTab="1" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
+    <workbookView xWindow="12120" yWindow="1460" windowWidth="23320" windowHeight="16680" activeTab="2" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
     <sheet name="openAccount" sheetId="2" r:id="rId2"/>
+    <sheet name="findCarTest" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -74,6 +75,30 @@
   </si>
   <si>
     <t>Ranbir Kapoor</t>
+  </si>
+  <si>
+    <t>brandName</t>
+  </si>
+  <si>
+    <t>Maruti</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>Hynundai</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>browserName</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
   </si>
 </sst>
 </file>
@@ -487,7 +512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77823ECE-AFC3-AA40-B1CB-0BC156BAA1BA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -532,4 +557,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BBD9E6-341F-4242-9B09-47697F6D6741}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fetching Model Name and Model Prices for each car brands
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rimadas/eclipse-workspace/SeleniumPageObjectModelFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B03991-E471-F54F-A3CC-48A0FF32A590}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E4C65B-2A6C-7141-9B06-A85E837F003E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="1460" windowWidth="23320" windowHeight="16680" activeTab="2" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
+    <workbookView xWindow="12120" yWindow="1460" windowWidth="23320" windowHeight="16680" activeTab="3" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
     <sheet name="openAccount" sheetId="2" r:id="rId2"/>
     <sheet name="findCarTest" sheetId="3" r:id="rId3"/>
+    <sheet name="findCarModelAndPriceTest" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -563,8 +564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BBD9E6-341F-4242-9B09-47697F6D6741}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -612,4 +613,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F44B0A-94E4-5940-8258-4270A66BA7B7}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding homePagetest to test the homepage
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rimadas/eclipse-workspace/SeleniumPageObjectModelFramework/src/test/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70E4C65B-2A6C-7141-9B06-A85E837F003E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E809DCE-5339-F84B-855A-79B3851D4CDD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12120" yWindow="1460" windowWidth="23320" windowHeight="16680" activeTab="3" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
+    <workbookView xWindow="12120" yWindow="1460" windowWidth="23320" windowHeight="16680" activeTab="4" xr2:uid="{3ADA70C4-690B-F340-9622-597162287630}"/>
   </bookViews>
   <sheets>
     <sheet name="addCustomer" sheetId="1" r:id="rId1"/>
     <sheet name="openAccount" sheetId="2" r:id="rId2"/>
     <sheet name="findCarTest" sheetId="3" r:id="rId3"/>
     <sheet name="findCarModelAndPriceTest" sheetId="4" r:id="rId4"/>
+    <sheet name="homePageTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>FirstName</t>
   </si>
@@ -619,8 +620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F44B0A-94E4-5940-8258-4270A66BA7B7}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -651,7 +652,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -659,10 +660,35 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D6E0CEB-0A43-074F-A064-C7BF4FCA0FA9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>